<commit_message>
memperbaiki struktur table user, dari prodi menjadi tingkat
</commit_message>
<xml_diff>
--- a/public/example-import/example_file.xlsx
+++ b/public/example-import/example_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A934C8-6124-4AF9-A5BF-187539A71C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910788CF-EF72-4C0D-B64F-DBBBAFD62953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>No</t>
   </si>
@@ -74,6 +74,18 @@
   </si>
   <si>
     <t>1EG4</t>
+  </si>
+  <si>
+    <t>Tingkat (Opsional)</t>
+  </si>
+  <si>
+    <t>Tingkat IV</t>
+  </si>
+  <si>
+    <t>Tingkat III</t>
+  </si>
+  <si>
+    <t>Tingkat I</t>
   </si>
 </sst>
 </file>
@@ -463,25 +475,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="5"/>
-    <col min="2" max="2" width="37.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6328125" style="1" customWidth="1"/>
     <col min="3" max="3" width="27" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.1796875" style="1" customWidth="1"/>
     <col min="5" max="5" width="22.54296875" style="1" customWidth="1"/>
     <col min="6" max="6" width="17.7265625" style="1" customWidth="1"/>
     <col min="7" max="7" width="19.6328125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="1"/>
+    <col min="8" max="8" width="18.54296875" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1">
+    <row r="1" spans="1:8" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -503,8 +516,11 @@
       <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -526,8 +542,11 @@
       <c r="G2" s="1">
         <v>61</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -547,8 +566,11 @@
       <c r="G3" s="1">
         <v>62</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -567,8 +589,11 @@
       <c r="G4" s="1">
         <v>63</v>
       </c>
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -586,6 +611,12 @@
       </c>
       <c r="F5" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="G5" s="1">
+        <v>64</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>